<commit_message>
Stop tracking myvenv_new virtual environment
</commit_message>
<xml_diff>
--- a/Innovius Task Sheet.xlsx
+++ b/Innovius Task Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5e644f5f8373b0ff/Desktop/Innovius/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="11_0FDEB5F77C09D11FF0CAF84DE1F38DA43D9943A8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F702F93D-6317-419D-B358-E377765F51E0}"/>
+  <xr:revisionPtr revIDLastSave="85" documentId="11_0FDEB5F77C09D11FF0CAF84DE1F38DA43D9943A8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2FCC3A65-5D3A-4589-AB30-708E7BC531F8}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
   <si>
     <t>Task Type</t>
   </si>
@@ -162,6 +162,18 @@
   </si>
   <si>
     <t>kishore sir</t>
+  </si>
+  <si>
+    <t>Installed required NLP techniques liky spaCy, scispacy, and pretrained models like en_core_sci_sm, en_core_web_sm. Built a Flask app and UI for the input and output of extracted features from the input text(medical features).</t>
+  </si>
+  <si>
+    <t>Developed a text classification model for categorizing patient records by disease type. And built a Flask app for the UI rendering.</t>
+  </si>
+  <si>
+    <t>incomplete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Build the UI using HTML/CSS for symptoms input and  predicting disease as output. Tested the model and worked fine. </t>
   </si>
 </sst>
 </file>
@@ -209,7 +221,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -232,11 +244,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -248,6 +271,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="F7" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -688,6 +714,92 @@
         <v>18</v>
       </c>
     </row>
+    <row r="6" spans="1:11" ht="58" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="4">
+        <v>45756</v>
+      </c>
+      <c r="J6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>30</v>
+      </c>
+      <c r="H7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="4">
+        <v>45756</v>
+      </c>
+      <c r="J7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="4">
+        <v>45757</v>
+      </c>
+      <c r="J8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>